<commit_message>
Emailing bacs creating month report and sending month end report code implementation done
</commit_message>
<xml_diff>
--- a/SDLT Running Code/Taylor Bot/Data/config/Mapping file for fee earner.xlsx
+++ b/SDLT Running Code/Taylor Bot/Data/config/Mapping file for fee earner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Taylors\Taylor Bot\Data\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3EDDB2-5D24-4A42-A383-2CF097DFFA78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15444687-D6F4-4978-9F47-5A9863AB936E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{C3243024-DD66-447E-971A-974DC9971839}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
   <si>
     <t xml:space="preserve">Nicola Taylor                   </t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>Zoe Baverstock</t>
+  </si>
+  <si>
+    <t>Sandeep Chahil</t>
   </si>
 </sst>
 </file>
@@ -469,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F7E060F-3FF5-4053-A3E8-A2CF4EC7F91C}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G19" sqref="F18:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,6 +621,14 @@
         <v>15</v>
       </c>
     </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>